<commit_message>
Pre add manager IP & port
</commit_message>
<xml_diff>
--- a/eeprom_map.xlsx
+++ b/eeprom_map.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="46">
   <si>
     <t>Partition 1</t>
   </si>
@@ -147,6 +147,21 @@
   </si>
   <si>
     <t>byte</t>
+  </si>
+  <si>
+    <t>Manager IP 0</t>
+  </si>
+  <si>
+    <t>Manager IP 1</t>
+  </si>
+  <si>
+    <t>Manager IP 2</t>
+  </si>
+  <si>
+    <t>Manager IP 3</t>
+  </si>
+  <si>
+    <t>Manage IP to connect or Acces Point IP config</t>
   </si>
 </sst>
 </file>
@@ -177,7 +192,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -280,6 +295,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -293,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -306,25 +333,27 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -605,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN26"/>
+  <dimension ref="A1:AN48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AH14" sqref="AH14"/>
+      <selection activeCell="AO34" sqref="AO34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,7 +649,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A1" s="18">
+      <c r="A1" s="14">
         <v>0</v>
       </c>
       <c r="B1" s="11">
@@ -629,83 +658,83 @@
       <c r="C1" s="10">
         <v>2</v>
       </c>
-      <c r="D1" s="20">
+      <c r="D1" s="16">
         <v>3</v>
       </c>
-      <c r="E1" s="20">
+      <c r="E1" s="16">
         <v>4</v>
       </c>
-      <c r="F1" s="20">
+      <c r="F1" s="16">
         <v>5</v>
       </c>
-      <c r="G1" s="20">
+      <c r="G1" s="16">
         <v>6</v>
       </c>
-      <c r="H1" s="20">
+      <c r="H1" s="16">
         <v>7</v>
       </c>
-      <c r="I1" s="20">
+      <c r="I1" s="16">
         <v>8</v>
       </c>
-      <c r="J1" s="22">
+      <c r="J1" s="18">
         <v>9</v>
       </c>
-      <c r="K1" s="22">
+      <c r="K1" s="18">
         <v>10</v>
       </c>
-      <c r="L1" s="19">
+      <c r="L1" s="15">
         <v>11</v>
       </c>
-      <c r="M1" s="19">
+      <c r="M1" s="15">
         <v>12</v>
       </c>
-      <c r="N1" s="19">
+      <c r="N1" s="15">
         <v>13</v>
       </c>
-      <c r="O1" s="19">
+      <c r="O1" s="15">
         <v>14</v>
       </c>
-      <c r="P1" s="19">
+      <c r="P1" s="15">
         <v>15</v>
       </c>
-      <c r="Q1" s="19">
+      <c r="Q1" s="15">
         <v>16</v>
       </c>
-      <c r="R1" s="22">
+      <c r="R1" s="18">
         <v>17</v>
       </c>
-      <c r="S1" s="22">
+      <c r="S1" s="18">
         <v>18</v>
       </c>
-      <c r="T1">
+      <c r="T1" s="23">
         <v>19</v>
       </c>
-      <c r="U1">
+      <c r="U1" s="23">
         <v>20</v>
       </c>
-      <c r="V1">
+      <c r="V1" s="23">
         <v>21</v>
       </c>
-      <c r="W1">
+      <c r="W1" s="23">
         <v>22</v>
       </c>
-      <c r="X1">
+      <c r="X1" s="24">
         <v>23</v>
       </c>
-      <c r="Y1">
+      <c r="Y1" s="24">
         <v>24</v>
       </c>
-      <c r="Z1" s="13" t="s">
+      <c r="Z1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="AB1" s="12" t="s">
+      <c r="AB1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="AC1" s="12"/>
-      <c r="AE1" s="12" t="s">
+      <c r="AC1" s="21"/>
+      <c r="AE1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="AF1" s="12"/>
+      <c r="AF1" s="21"/>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -783,27 +812,27 @@
       <c r="Y2">
         <v>49</v>
       </c>
-      <c r="Z2" s="13"/>
-      <c r="AB2" s="4" t="s">
-        <v>13</v>
+      <c r="Z2" s="20"/>
+      <c r="AB2" s="14" t="s">
+        <v>32</v>
       </c>
       <c r="AC2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE2" s="5" t="s">
-        <v>13</v>
+        <v>5</v>
+      </c>
+      <c r="AE2" s="9" t="s">
+        <v>32</v>
       </c>
       <c r="AF2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI2" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="AJ2" s="16"/>
-      <c r="AK2" s="16"/>
-      <c r="AL2" s="16"/>
-      <c r="AM2" s="16"/>
-      <c r="AN2" s="16"/>
+        <v>5</v>
+      </c>
+      <c r="AI2" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ2" s="19"/>
+      <c r="AK2" s="19"/>
+      <c r="AL2" s="19"/>
+      <c r="AM2" s="19"/>
+      <c r="AN2" s="19"/>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
@@ -881,27 +910,27 @@
       <c r="Y3" s="4">
         <v>74</v>
       </c>
-      <c r="Z3" s="13"/>
-      <c r="AB3" s="3" t="s">
-        <v>13</v>
+      <c r="Z3" s="20"/>
+      <c r="AB3" s="14" t="s">
+        <v>33</v>
       </c>
       <c r="AC3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AE3" s="2" t="s">
-        <v>13</v>
+        <v>29</v>
+      </c>
+      <c r="AE3" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="AF3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AI3" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="AJ3" s="16"/>
-      <c r="AK3" s="16"/>
-      <c r="AL3" s="16"/>
-      <c r="AM3" s="16"/>
-      <c r="AN3" s="16"/>
+        <v>29</v>
+      </c>
+      <c r="AI3" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="AJ3" s="19"/>
+      <c r="AK3" s="19"/>
+      <c r="AL3" s="19"/>
+      <c r="AM3" s="19"/>
+      <c r="AN3" s="19"/>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
@@ -979,27 +1008,13 @@
       <c r="Y4" s="4">
         <v>99</v>
       </c>
-      <c r="Z4" s="13"/>
+      <c r="Z4" s="20"/>
       <c r="AB4" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>4</v>
-      </c>
-      <c r="AE4" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>4</v>
-      </c>
-      <c r="AI4" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="AJ4" s="16"/>
-      <c r="AK4" s="16"/>
-      <c r="AL4" s="16"/>
-      <c r="AM4" s="16"/>
-      <c r="AN4" s="16"/>
+        <v>34</v>
+      </c>
+      <c r="AE4" s="9" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
@@ -1077,27 +1092,13 @@
       <c r="Y5" s="4">
         <v>124</v>
       </c>
-      <c r="Z5" s="13"/>
-      <c r="AB5" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>5</v>
+      <c r="Z5" s="20"/>
+      <c r="AB5" s="14" t="s">
+        <v>35</v>
       </c>
       <c r="AE5" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI5" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ5" s="16"/>
-      <c r="AK5" s="16"/>
-      <c r="AL5" s="16"/>
-      <c r="AM5" s="16"/>
-      <c r="AN5" s="16"/>
+        <v>35</v>
+      </c>
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
@@ -1175,27 +1176,13 @@
       <c r="Y6" s="4">
         <v>149</v>
       </c>
-      <c r="Z6" s="13"/>
-      <c r="AB6" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>29</v>
+      <c r="Z6" s="20"/>
+      <c r="AB6" s="14" t="s">
+        <v>36</v>
       </c>
       <c r="AE6" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="AF6" t="s">
-        <v>29</v>
-      </c>
-      <c r="AI6" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="AJ6" s="16"/>
-      <c r="AK6" s="16"/>
-      <c r="AL6" s="16"/>
-      <c r="AM6" s="16"/>
-      <c r="AN6" s="16"/>
+        <v>36</v>
+      </c>
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
@@ -1273,12 +1260,12 @@
       <c r="Y7" s="3">
         <v>174</v>
       </c>
-      <c r="Z7" s="13"/>
-      <c r="AB7" s="18" t="s">
-        <v>34</v>
+      <c r="Z7" s="20"/>
+      <c r="AB7" s="14" t="s">
+        <v>37</v>
       </c>
       <c r="AE7" s="9" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.25">
@@ -1357,12 +1344,12 @@
       <c r="Y8" s="3">
         <v>199</v>
       </c>
-      <c r="Z8" s="13"/>
-      <c r="AB8" s="18" t="s">
-        <v>35</v>
+      <c r="Z8" s="20"/>
+      <c r="AB8" s="14" t="s">
+        <v>38</v>
       </c>
       <c r="AE8" s="9" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.25">
@@ -1441,12 +1428,12 @@
       <c r="Y9" s="3">
         <v>224</v>
       </c>
-      <c r="Z9" s="13"/>
-      <c r="AB9" s="18" t="s">
-        <v>36</v>
+      <c r="Z9" s="20"/>
+      <c r="AB9" s="14" t="s">
+        <v>39</v>
       </c>
       <c r="AE9" s="9" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:40" x14ac:dyDescent="0.25">
@@ -1525,13 +1512,27 @@
       <c r="Y10" s="3">
         <v>249</v>
       </c>
-      <c r="Z10" s="13"/>
-      <c r="AB10" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="AE10" s="9" t="s">
-        <v>37</v>
-      </c>
+      <c r="Z10" s="20"/>
+      <c r="AB10" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE10" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>6</v>
+      </c>
+      <c r="AI10" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="AJ10" s="19"/>
+      <c r="AK10" s="19"/>
+      <c r="AL10" s="19"/>
+      <c r="AM10" s="19"/>
+      <c r="AN10" s="19"/>
     </row>
     <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
@@ -1540,7 +1541,7 @@
       <c r="B11" s="6">
         <v>251</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C11" s="17">
         <v>252</v>
       </c>
       <c r="D11" s="8">
@@ -1561,10 +1562,10 @@
       <c r="I11" s="8">
         <v>258</v>
       </c>
-      <c r="J11" s="22">
+      <c r="J11" s="18">
         <v>259</v>
       </c>
-      <c r="K11" s="22">
+      <c r="K11" s="18">
         <v>260</v>
       </c>
       <c r="L11" s="7">
@@ -1585,10 +1586,10 @@
       <c r="Q11" s="7">
         <v>266</v>
       </c>
-      <c r="R11" s="22">
+      <c r="R11" s="18">
         <v>267</v>
       </c>
-      <c r="S11" s="22">
+      <c r="S11" s="18">
         <v>268</v>
       </c>
       <c r="T11">
@@ -1609,15 +1610,29 @@
       <c r="Y11">
         <v>274</v>
       </c>
-      <c r="Z11" s="13" t="s">
+      <c r="Z11" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="AB11" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="AE11" s="9" t="s">
-        <v>38</v>
-      </c>
+      <c r="AB11" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE11" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI11" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ11" s="19"/>
+      <c r="AK11" s="19"/>
+      <c r="AL11" s="19"/>
+      <c r="AM11" s="19"/>
+      <c r="AN11" s="19"/>
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1695,13 +1710,27 @@
       <c r="Y12">
         <v>299</v>
       </c>
-      <c r="Z12" s="13"/>
-      <c r="AB12" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="AE12" s="9" t="s">
-        <v>39</v>
-      </c>
+      <c r="Z12" s="20"/>
+      <c r="AB12" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE12" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI12" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="AJ12" s="22"/>
+      <c r="AK12" s="22"/>
+      <c r="AL12" s="22"/>
+      <c r="AM12" s="22"/>
+      <c r="AN12" s="22"/>
     </row>
     <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
@@ -1779,27 +1808,25 @@
       <c r="Y13" s="5">
         <v>324</v>
       </c>
-      <c r="Z13" s="13"/>
-      <c r="AB13" s="11" t="s">
+      <c r="Z13" s="20"/>
+      <c r="AB13" s="16" t="s">
         <v>40</v>
       </c>
       <c r="AC13" t="s">
-        <v>6</v>
-      </c>
-      <c r="AE13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE13" s="8" t="s">
         <v>40</v>
       </c>
       <c r="AF13" t="s">
-        <v>6</v>
-      </c>
-      <c r="AI13" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="AJ13" s="16"/>
-      <c r="AK13" s="16"/>
-      <c r="AL13" s="16"/>
-      <c r="AM13" s="16"/>
-      <c r="AN13" s="16"/>
+        <v>16</v>
+      </c>
+      <c r="AI13" s="22"/>
+      <c r="AJ13" s="22"/>
+      <c r="AK13" s="22"/>
+      <c r="AL13" s="22"/>
+      <c r="AM13" s="22"/>
+      <c r="AN13" s="22"/>
     </row>
     <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
@@ -1877,27 +1904,25 @@
       <c r="Y14" s="5">
         <v>349</v>
       </c>
-      <c r="Z14" s="13"/>
-      <c r="AB14" s="10" t="s">
+      <c r="Z14" s="20"/>
+      <c r="AB14" s="16" t="s">
         <v>40</v>
       </c>
       <c r="AC14" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE14" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="AE14" s="8" t="s">
         <v>40</v>
       </c>
       <c r="AF14" t="s">
-        <v>12</v>
-      </c>
-      <c r="AI14" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ14" s="16"/>
-      <c r="AK14" s="16"/>
-      <c r="AL14" s="16"/>
-      <c r="AM14" s="16"/>
-      <c r="AN14" s="16"/>
+        <v>17</v>
+      </c>
+      <c r="AI14" s="22"/>
+      <c r="AJ14" s="22"/>
+      <c r="AK14" s="22"/>
+      <c r="AL14" s="22"/>
+      <c r="AM14" s="22"/>
+      <c r="AN14" s="22"/>
     </row>
     <row r="15" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
@@ -1975,27 +2000,25 @@
       <c r="Y15" s="5">
         <v>374</v>
       </c>
-      <c r="Z15" s="13"/>
-      <c r="AB15" s="20" t="s">
+      <c r="Z15" s="20"/>
+      <c r="AB15" s="16" t="s">
         <v>40</v>
       </c>
       <c r="AC15" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="AE15" s="8" t="s">
         <v>40</v>
       </c>
       <c r="AF15" t="s">
-        <v>15</v>
-      </c>
-      <c r="AI15" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="AJ15" s="17"/>
-      <c r="AK15" s="17"/>
-      <c r="AL15" s="17"/>
-      <c r="AM15" s="17"/>
-      <c r="AN15" s="17"/>
+        <v>18</v>
+      </c>
+      <c r="AI15" s="22"/>
+      <c r="AJ15" s="22"/>
+      <c r="AK15" s="22"/>
+      <c r="AL15" s="22"/>
+      <c r="AM15" s="22"/>
+      <c r="AN15" s="22"/>
     </row>
     <row r="16" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
@@ -2073,25 +2096,25 @@
       <c r="Y16" s="5">
         <v>399</v>
       </c>
-      <c r="Z16" s="13"/>
-      <c r="AB16" s="20" t="s">
+      <c r="Z16" s="20"/>
+      <c r="AB16" s="16" t="s">
         <v>40</v>
       </c>
       <c r="AC16" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="AE16" s="8" t="s">
         <v>40</v>
       </c>
       <c r="AF16" t="s">
-        <v>16</v>
-      </c>
-      <c r="AI16" s="17"/>
-      <c r="AJ16" s="17"/>
-      <c r="AK16" s="17"/>
-      <c r="AL16" s="17"/>
-      <c r="AM16" s="17"/>
-      <c r="AN16" s="17"/>
+        <v>19</v>
+      </c>
+      <c r="AI16" s="22"/>
+      <c r="AJ16" s="22"/>
+      <c r="AK16" s="22"/>
+      <c r="AL16" s="22"/>
+      <c r="AM16" s="22"/>
+      <c r="AN16" s="22"/>
     </row>
     <row r="17" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
@@ -2169,25 +2192,25 @@
       <c r="Y17" s="2">
         <v>424</v>
       </c>
-      <c r="Z17" s="13"/>
-      <c r="AB17" s="20" t="s">
+      <c r="Z17" s="20"/>
+      <c r="AB17" s="16" t="s">
         <v>40</v>
       </c>
       <c r="AC17" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="AE17" s="8" t="s">
         <v>40</v>
       </c>
       <c r="AF17" t="s">
-        <v>17</v>
-      </c>
-      <c r="AI17" s="17"/>
-      <c r="AJ17" s="17"/>
-      <c r="AK17" s="17"/>
-      <c r="AL17" s="17"/>
-      <c r="AM17" s="17"/>
-      <c r="AN17" s="17"/>
+        <v>20</v>
+      </c>
+      <c r="AI17" s="22"/>
+      <c r="AJ17" s="22"/>
+      <c r="AK17" s="22"/>
+      <c r="AL17" s="22"/>
+      <c r="AM17" s="22"/>
+      <c r="AN17" s="22"/>
     </row>
     <row r="18" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
@@ -2265,25 +2288,7 @@
       <c r="Y18" s="2">
         <v>449</v>
       </c>
-      <c r="Z18" s="13"/>
-      <c r="AB18" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC18" t="s">
-        <v>18</v>
-      </c>
-      <c r="AE18" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="AF18" t="s">
-        <v>18</v>
-      </c>
-      <c r="AI18" s="17"/>
-      <c r="AJ18" s="17"/>
-      <c r="AK18" s="17"/>
-      <c r="AL18" s="17"/>
-      <c r="AM18" s="17"/>
-      <c r="AN18" s="17"/>
+      <c r="Z18" s="20"/>
     </row>
     <row r="19" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
@@ -2361,25 +2366,7 @@
       <c r="Y19" s="2">
         <v>474</v>
       </c>
-      <c r="Z19" s="13"/>
-      <c r="AB19" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC19" t="s">
-        <v>19</v>
-      </c>
-      <c r="AE19" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="AF19" t="s">
-        <v>19</v>
-      </c>
-      <c r="AI19" s="17"/>
-      <c r="AJ19" s="17"/>
-      <c r="AK19" s="17"/>
-      <c r="AL19" s="17"/>
-      <c r="AM19" s="17"/>
-      <c r="AN19" s="17"/>
+      <c r="Z19" s="20"/>
     </row>
     <row r="20" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
@@ -2457,25 +2444,27 @@
       <c r="Y20" s="2">
         <v>499</v>
       </c>
-      <c r="Z20" s="13"/>
-      <c r="AB20" s="20" t="s">
+      <c r="Z20" s="20"/>
+      <c r="AB20" s="15" t="s">
         <v>40</v>
       </c>
       <c r="AC20" t="s">
-        <v>20</v>
-      </c>
-      <c r="AE20" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE20" s="7" t="s">
         <v>40</v>
       </c>
       <c r="AF20" t="s">
-        <v>20</v>
-      </c>
-      <c r="AI20" s="17"/>
-      <c r="AJ20" s="17"/>
-      <c r="AK20" s="17"/>
-      <c r="AL20" s="17"/>
-      <c r="AM20" s="17"/>
-      <c r="AN20" s="17"/>
+        <v>21</v>
+      </c>
+      <c r="AI20" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="AJ20" s="22"/>
+      <c r="AK20" s="22"/>
+      <c r="AL20" s="22"/>
+      <c r="AM20" s="22"/>
+      <c r="AN20" s="22"/>
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A21">
@@ -2490,167 +2479,280 @@
       <c r="D21">
         <v>503</v>
       </c>
-      <c r="E21" s="14">
+      <c r="E21" s="12">
         <v>504</v>
       </c>
-      <c r="F21" s="14">
+      <c r="F21" s="12">
         <v>505</v>
       </c>
-      <c r="G21" s="14">
+      <c r="G21" s="12">
         <v>506</v>
       </c>
-      <c r="H21" s="14">
+      <c r="H21" s="12">
         <v>507</v>
       </c>
-      <c r="I21" s="15">
+      <c r="I21" s="13">
         <v>508</v>
       </c>
-      <c r="J21" s="15">
+      <c r="J21" s="13">
         <v>509</v>
       </c>
-      <c r="K21" s="15">
+      <c r="K21" s="13">
         <v>510</v>
       </c>
-      <c r="L21" s="15">
+      <c r="L21" s="13">
         <v>511</v>
       </c>
-      <c r="AB21" s="20" t="s">
+      <c r="AB21" s="15" t="s">
         <v>40</v>
       </c>
       <c r="AC21" t="s">
-        <v>21</v>
-      </c>
-      <c r="AE21" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE21" s="7" t="s">
         <v>40</v>
       </c>
       <c r="AF21" t="s">
-        <v>21</v>
-      </c>
-      <c r="AI21" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="AJ21" s="17"/>
-      <c r="AK21" s="17"/>
-      <c r="AL21" s="17"/>
-      <c r="AM21" s="17"/>
-      <c r="AN21" s="17"/>
+        <v>22</v>
+      </c>
+      <c r="AI21" s="22"/>
+      <c r="AJ21" s="22"/>
+      <c r="AK21" s="22"/>
+      <c r="AL21" s="22"/>
+      <c r="AM21" s="22"/>
+      <c r="AN21" s="22"/>
     </row>
     <row r="22" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="AB22" s="20" t="s">
+      <c r="AB22" s="15" t="s">
         <v>40</v>
       </c>
       <c r="AC22" t="s">
-        <v>22</v>
-      </c>
-      <c r="AE22" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE22" s="7" t="s">
         <v>40</v>
       </c>
       <c r="AF22" t="s">
-        <v>22</v>
-      </c>
-      <c r="AI22" s="17"/>
-      <c r="AJ22" s="17"/>
-      <c r="AK22" s="17"/>
-      <c r="AL22" s="17"/>
-      <c r="AM22" s="17"/>
-      <c r="AN22" s="17"/>
+        <v>23</v>
+      </c>
+      <c r="AI22" s="22"/>
+      <c r="AJ22" s="22"/>
+      <c r="AK22" s="22"/>
+      <c r="AL22" s="22"/>
+      <c r="AM22" s="22"/>
+      <c r="AN22" s="22"/>
     </row>
     <row r="23" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="AB23" s="20" t="s">
+      <c r="AB23" s="15" t="s">
         <v>40</v>
       </c>
       <c r="AC23" t="s">
-        <v>23</v>
-      </c>
-      <c r="AE23" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE23" s="7" t="s">
         <v>40</v>
       </c>
       <c r="AF23" t="s">
-        <v>23</v>
-      </c>
-      <c r="AI23" s="17"/>
-      <c r="AJ23" s="17"/>
-      <c r="AK23" s="17"/>
-      <c r="AL23" s="17"/>
-      <c r="AM23" s="17"/>
-      <c r="AN23" s="17"/>
+        <v>24</v>
+      </c>
+      <c r="AI23" s="22"/>
+      <c r="AJ23" s="22"/>
+      <c r="AK23" s="22"/>
+      <c r="AL23" s="22"/>
+      <c r="AM23" s="22"/>
+      <c r="AN23" s="22"/>
     </row>
     <row r="24" spans="1:40" x14ac:dyDescent="0.25">
       <c r="W24" s="1"/>
-      <c r="AB24" s="20" t="s">
+      <c r="AB24" s="15" t="s">
         <v>40</v>
       </c>
       <c r="AC24" t="s">
-        <v>24</v>
-      </c>
-      <c r="AE24" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE24" s="7" t="s">
         <v>40</v>
       </c>
       <c r="AF24" t="s">
-        <v>24</v>
-      </c>
-      <c r="AI24" s="17"/>
-      <c r="AJ24" s="17"/>
-      <c r="AK24" s="17"/>
-      <c r="AL24" s="17"/>
-      <c r="AM24" s="17"/>
-      <c r="AN24" s="17"/>
+        <v>25</v>
+      </c>
+      <c r="AI24" s="22"/>
+      <c r="AJ24" s="22"/>
+      <c r="AK24" s="22"/>
+      <c r="AL24" s="22"/>
+      <c r="AM24" s="22"/>
+      <c r="AN24" s="22"/>
     </row>
     <row r="25" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="AB25" s="20" t="s">
+      <c r="AB25" s="15" t="s">
         <v>40</v>
       </c>
       <c r="AC25" t="s">
-        <v>25</v>
-      </c>
-      <c r="AE25" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE25" s="7" t="s">
         <v>40</v>
       </c>
       <c r="AF25" t="s">
-        <v>25</v>
-      </c>
-      <c r="AI25" s="17"/>
-      <c r="AJ25" s="17"/>
-      <c r="AK25" s="17"/>
-      <c r="AL25" s="17"/>
-      <c r="AM25" s="17"/>
-      <c r="AN25" s="17"/>
-    </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="AB26" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC26" t="s">
         <v>26</v>
       </c>
-      <c r="AE26" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="AF26" t="s">
-        <v>26</v>
-      </c>
-      <c r="AI26" s="17"/>
-      <c r="AJ26" s="17"/>
-      <c r="AK26" s="17"/>
-      <c r="AL26" s="17"/>
-      <c r="AM26" s="17"/>
-      <c r="AN26" s="17"/>
+      <c r="AI25" s="22"/>
+      <c r="AJ25" s="22"/>
+      <c r="AK25" s="22"/>
+      <c r="AL25" s="22"/>
+      <c r="AM25" s="22"/>
+      <c r="AN25" s="22"/>
+    </row>
+    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AB28" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC28" t="s">
+        <v>41</v>
+      </c>
+      <c r="AI28" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="AJ28" s="22"/>
+      <c r="AK28" s="22"/>
+      <c r="AL28" s="22"/>
+      <c r="AM28" s="22"/>
+      <c r="AN28" s="22"/>
+    </row>
+    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AB29" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC29" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI29" s="22"/>
+      <c r="AJ29" s="22"/>
+      <c r="AK29" s="22"/>
+      <c r="AL29" s="22"/>
+      <c r="AM29" s="22"/>
+      <c r="AN29" s="22"/>
+    </row>
+    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AB30" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC30" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI30" s="22"/>
+      <c r="AJ30" s="22"/>
+      <c r="AK30" s="22"/>
+      <c r="AL30" s="22"/>
+      <c r="AM30" s="22"/>
+      <c r="AN30" s="22"/>
+    </row>
+    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AB31" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC31" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI31" s="22"/>
+      <c r="AJ31" s="22"/>
+      <c r="AK31" s="22"/>
+      <c r="AL31" s="22"/>
+      <c r="AM31" s="22"/>
+      <c r="AN31" s="22"/>
+    </row>
+    <row r="32" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AB32" s="24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="28:40" x14ac:dyDescent="0.25">
+      <c r="AB33" s="24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46" spans="28:40" x14ac:dyDescent="0.25">
+      <c r="AB46" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC46" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE46" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF46" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI46" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ46" s="19"/>
+      <c r="AK46" s="19"/>
+      <c r="AL46" s="19"/>
+      <c r="AM46" s="19"/>
+      <c r="AN46" s="19"/>
+    </row>
+    <row r="47" spans="28:40" x14ac:dyDescent="0.25">
+      <c r="AB47" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC47" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE47" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF47" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI47" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ47" s="19"/>
+      <c r="AK47" s="19"/>
+      <c r="AL47" s="19"/>
+      <c r="AM47" s="19"/>
+      <c r="AN47" s="19"/>
+    </row>
+    <row r="48" spans="28:40" x14ac:dyDescent="0.25">
+      <c r="AB48" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC48" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE48" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF48" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI48" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="AJ48" s="19"/>
+      <c r="AK48" s="19"/>
+      <c r="AL48" s="19"/>
+      <c r="AM48" s="19"/>
+      <c r="AN48" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="AI2:AN2"/>
-    <mergeCell ref="AI3:AN3"/>
-    <mergeCell ref="AI4:AN4"/>
-    <mergeCell ref="AI6:AN6"/>
-    <mergeCell ref="Z1:Z10"/>
+  <mergeCells count="14">
     <mergeCell ref="Z11:Z20"/>
     <mergeCell ref="AB1:AC1"/>
     <mergeCell ref="AE1:AF1"/>
-    <mergeCell ref="AI15:AN20"/>
-    <mergeCell ref="AI21:AN26"/>
-    <mergeCell ref="AI5:AN5"/>
-    <mergeCell ref="AI14:AN14"/>
-    <mergeCell ref="AI13:AN13"/>
+    <mergeCell ref="AI12:AN17"/>
+    <mergeCell ref="AI20:AN25"/>
+    <mergeCell ref="AI11:AN11"/>
+    <mergeCell ref="AI10:AN10"/>
+    <mergeCell ref="AI2:AN2"/>
+    <mergeCell ref="AI3:AN3"/>
+    <mergeCell ref="AI46:AN46"/>
+    <mergeCell ref="AI47:AN47"/>
+    <mergeCell ref="AI48:AN48"/>
+    <mergeCell ref="Z1:Z10"/>
+    <mergeCell ref="AI28:AN31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>